<commit_message>
Update Excel letterhead template
</commit_message>
<xml_diff>
--- a/public/templates/letter-head.xlsx
+++ b/public/templates/letter-head.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10201"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E6DA645-AC43-5A4E-9A09-38A50053A672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8EF3A2-E455-EC47-9569-3F694360651C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -72,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -93,46 +89,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -172,88 +128,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -271,79 +150,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,28 +1040,21 @@
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t> : 14</a:t>
+            <a:t> : 00</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>/05</a:t>
+            <a:t>/00</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-IN" sz="1100" b="1" baseline="0">
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>/202</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>4</a:t>
+            <a:t>/2026</a:t>
           </a:r>
           <a:endParaRPr lang="en-IN" sz="1100" b="1">
             <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
@@ -1544,312 +1369,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="32"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="28"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="26"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1857,12 +1682,12 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -1870,12 +1695,12 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -1883,12 +1708,12 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -1896,12 +1721,12 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -1909,12 +1734,12 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
@@ -1922,12 +1747,12 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -1935,12 +1760,12 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -1948,12 +1773,12 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -1961,51 +1786,51 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="28"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="28"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="28"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
@@ -2013,12 +1838,12 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
@@ -2103,34 +1928,12 @@
       <c r="K43" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="5">
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
     <mergeCell ref="A1:K12"/>
     <mergeCell ref="A13:K13"/>
     <mergeCell ref="B14:G14"/>
-    <mergeCell ref="I15:I22"/>
-    <mergeCell ref="J15:J22"/>
-    <mergeCell ref="K15:K22"/>
-    <mergeCell ref="H15:H22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B15:G22"/>
-    <mergeCell ref="A15:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>